<commit_message>
Added excel upload changes
</commit_message>
<xml_diff>
--- a/Documents/EmployeeInsertTemplate.xlsx
+++ b/Documents/EmployeeInsertTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chatt\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC247BEC-50E8-43DC-869E-DB5224A99846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50BCE85D-7E9B-4968-8C47-03D8E104E4A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B0448C85-CBD7-4AC4-AC87-8AA559B26FD2}"/>
   </bookViews>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
-  <si>
-    <t>CompanyId</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Role</t>
   </si>
@@ -44,9 +41,6 @@
     <t>Group</t>
   </si>
   <si>
-    <t>Designation</t>
-  </si>
-  <si>
     <t>First Name</t>
   </si>
   <si>
@@ -71,64 +65,19 @@
     <t>DOR</t>
   </si>
   <si>
-    <t>Assets</t>
-  </si>
-  <si>
     <t>OverdueApprovalDate</t>
   </si>
   <si>
-    <t>6C0276EC-FEA1-4FA8-BB1F-5D428A850222</t>
-  </si>
-  <si>
-    <t>6C0276EC-FEA1-4FA8-BB1F-9D228A850201</t>
-  </si>
-  <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>L2</t>
-  </si>
-  <si>
-    <t>L3</t>
-  </si>
-  <si>
-    <t>L4</t>
-  </si>
-  <si>
-    <t>Mirza</t>
-  </si>
-  <si>
-    <t>maig</t>
-  </si>
-  <si>
-    <t>Ankita</t>
-  </si>
-  <si>
-    <t>bedi</t>
-  </si>
-  <si>
-    <t>Ravi</t>
-  </si>
-  <si>
-    <t>Nigam</t>
-  </si>
-  <si>
     <t>Jason</t>
   </si>
   <si>
     <t>Thomas</t>
   </si>
   <si>
-    <t>Test1@gmail.com</t>
-  </si>
-  <si>
-    <t>Test2@gmail.com</t>
-  </si>
-  <si>
-    <t>Test3@gmail.com</t>
-  </si>
-  <si>
-    <t>Test4@gmail.com</t>
+    <t>Jthomson@crossleaf.com</t>
+  </si>
+  <si>
+    <t>Developer</t>
   </si>
 </sst>
 </file>
@@ -537,27 +486,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BA8E9CB-7112-4B55-867F-B12215CC3947}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.77734375" customWidth="1"/>
-    <col min="2" max="2" width="37" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" customWidth="1"/>
-    <col min="6" max="6" width="10.77734375" customWidth="1"/>
-    <col min="7" max="7" width="22.88671875" customWidth="1"/>
-    <col min="8" max="8" width="19" customWidth="1"/>
-    <col min="9" max="9" width="15.77734375" customWidth="1"/>
-    <col min="10" max="11" width="13.33203125" customWidth="1"/>
-    <col min="14" max="14" width="25.5546875" customWidth="1"/>
+    <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" customWidth="1"/>
+    <col min="5" max="5" width="22.88671875" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="7" max="7" width="15.77734375" customWidth="1"/>
+    <col min="8" max="9" width="13.33203125" customWidth="1"/>
+    <col min="11" max="11" width="25.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -591,177 +538,44 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="D2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" s="2">
-        <v>1234567890</v>
-      </c>
-      <c r="I2" s="2">
-        <v>9808991122</v>
-      </c>
-      <c r="J2" s="3">
-        <v>33024</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1234567893</v>
+      </c>
+      <c r="G2" s="2">
+        <v>9808991129</v>
+      </c>
+      <c r="H2" s="3">
+        <v>33027</v>
+      </c>
+      <c r="I2" s="3">
+        <v>40212</v>
+      </c>
+      <c r="J2" s="2"/>
       <c r="K2" s="3">
-        <v>40209</v>
-      </c>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="3">
-        <v>44676</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="2">
-        <v>1234567891</v>
-      </c>
-      <c r="I3" s="2">
-        <v>9808991125</v>
-      </c>
-      <c r="J3" s="3">
-        <v>33025</v>
-      </c>
-      <c r="K3" s="3">
-        <v>40210</v>
-      </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="3">
-        <v>44677</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="2">
-        <v>1234567892</v>
-      </c>
-      <c r="I4" s="2">
-        <v>9808991123</v>
-      </c>
-      <c r="J4" s="3">
-        <v>33026</v>
-      </c>
-      <c r="K4" s="3">
-        <v>40211</v>
-      </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="3">
-        <v>44678</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" s="2">
-        <v>1234567893</v>
-      </c>
-      <c r="I5" s="2">
-        <v>9808991129</v>
-      </c>
-      <c r="J5" s="3">
-        <v>33027</v>
-      </c>
-      <c r="K5" s="3">
-        <v>40212</v>
-      </c>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="3">
         <v>44679</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{0B4A8DB1-5FBF-4A6E-8D27-D6F47200DC7E}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{78878EC4-71E8-444D-A29A-941C0311A545}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{A8DBF197-02D2-4273-9F7F-13CD6BD88761}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{D03513F7-FCD3-433D-9A1F-30467354A326}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{D03513F7-FCD3-433D-9A1F-30467354A326}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>